<commit_message>
updated story.ni, updated Org-chart, included
</commit_message>
<xml_diff>
--- a/Game2500-rpg Org-chart.xlsx
+++ b/Game2500-rpg Org-chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://northeastern-my.sharepoint.com/personal/elsayed_s_northeastern_edu/Documents/Foundations of Game Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Documents\GitHub\GAME2500-RPG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3C885DA-7DF8-4502-81C1-944F15A679B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63915F22-8A0F-4F42-AAA7-FA8FCD4089C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{529E1FA7-0718-4BDE-AE0F-699A3D90A599}"/>
+    <workbookView xWindow="3855" yWindow="2970" windowWidth="21600" windowHeight="11385" xr2:uid="{529E1FA7-0718-4BDE-AE0F-699A3D90A599}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Tenament</t>
   </si>
@@ -85,6 +85,45 @@
   </si>
   <si>
     <t>There to give you your lunch (for now)</t>
+  </si>
+  <si>
+    <t>Front Gate</t>
+  </si>
+  <si>
+    <t>Worker's Entrance</t>
+  </si>
+  <si>
+    <t>Main Entrance</t>
+  </si>
+  <si>
+    <t>Intake Desk</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>Spindle Room</t>
+  </si>
+  <si>
+    <t>Cotton Engines</t>
+  </si>
+  <si>
+    <t>Loading Dock</t>
+  </si>
+  <si>
+    <t>Central Stairs</t>
+  </si>
+  <si>
+    <t>Boiler Room</t>
+  </si>
+  <si>
+    <t>Finishing Room</t>
+  </si>
+  <si>
+    <t>Locker Rooms</t>
+  </si>
+  <si>
+    <t>Basement Stairs</t>
   </si>
 </sst>
 </file>
@@ -100,12 +139,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,8 +165,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{632947CF-8124-4195-B073-99209FB884B7}">
-  <dimension ref="G4:S13"/>
+  <dimension ref="G4:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,6 +506,10 @@
   </cols>
   <sheetData>
     <row r="4" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="4"/>
       <c r="P4" t="s">
         <v>4</v>
       </c>
@@ -509,37 +566,102 @@
       </c>
     </row>
     <row r="9" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
-        <v>2</v>
-      </c>
+      <c r="I9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="I10" t="s">
-        <v>3</v>
-      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="1"/>
       <c r="P10" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J11" s="1"/>
       <c r="P11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="1"/>
       <c r="P12" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="P13" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>